<commit_message>
fix can not get full data to value for exccell - laptop
</commit_message>
<xml_diff>
--- a/200 in4.xlsx
+++ b/200 in4.xlsx
@@ -1001,6 +1001,16 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>33-3950749</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>GAIL HINKEL</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
           <t>094484153</t>
@@ -1211,6 +1221,16 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>33-3950813</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DEMETRIC FORNEY</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>135643630</t>
@@ -1295,6 +1315,16 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>33-3950839</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ALLISON LEWIS</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
           <t>132625821</t>
@@ -1337,6 +1367,16 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>33-3950858</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DOMINGO SOTO</t>
+        </is>
+      </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
           <t>131506490</t>
@@ -1715,6 +1755,16 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>33-3951010</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>JUDY CRUZ PALMA</t>
+        </is>
+      </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
           <t>114704216</t>

</xml_diff>